<commit_message>
Update Tarefa2 Criação Fracao e TesteFracao
</commit_message>
<xml_diff>
--- a/LabDesenvolvimento/Tarefa2/Aplicação/TesteFracao.xlsx
+++ b/LabDesenvolvimento/Tarefa2/Aplicação/TesteFracao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvpau\Documents\GitHub\Jacinto\LabDesenvolvimento\Tarefa2\Aplicação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F809F799-DB3B-4D79-B968-32B1CAE66A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD14985-46C0-407B-B0F1-27C356FD82B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E56615B-2EBE-4CB0-A164-85E4DC1DF5F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Teste de Mesa - Fração</t>
   </si>
@@ -51,16 +51,86 @@
   </si>
   <si>
     <t>Numerador Segunda Fracao</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Equação</t>
+  </si>
+  <si>
+    <t>Divisão</t>
+  </si>
+  <si>
+    <r>
+      <t>15/4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>Subtração</t>
+  </si>
+  <si>
+    <r>
+      <t>29/35</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Multiplicação</t>
+  </si>
+  <si>
+    <r>
+      <t>35/12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,16 +156,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -437,73 +504,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B58EA01-7EAE-4A0D-8EC1-89D9053C8FCB}">
-  <dimension ref="C3:L6"/>
+  <dimension ref="B3:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="30.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.33203125" style="1" customWidth="1"/>
+    <col min="2" max="7" width="30.88671875" style="1" customWidth="1"/>
     <col min="8" max="12" width="14.109375" style="1" customWidth="1"/>
     <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="E7" s="1">
         <v>3</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C5" s="5">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="D5" s="5">
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
         <v>4</v>
       </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Tarefa2 Criação 4
</commit_message>
<xml_diff>
--- a/LabDesenvolvimento/Tarefa2/Aplicação/TesteFracao.xlsx
+++ b/LabDesenvolvimento/Tarefa2/Aplicação/TesteFracao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvpau\Documents\GitHub\Jacinto\LabDesenvolvimento\Tarefa2\Aplicação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD14985-46C0-407B-B0F1-27C356FD82B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F854A1-40FB-45FA-8E22-2820B96356E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E56615B-2EBE-4CB0-A164-85E4DC1DF5F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Teste de Mesa - Fração</t>
   </si>
@@ -114,6 +114,21 @@
       </rPr>
       <t>*</t>
     </r>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Método Recursivo</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>mdc</t>
+  </si>
+  <si>
+    <t>resto</t>
   </si>
 </sst>
 </file>
@@ -156,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -165,9 +180,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -504,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B58EA01-7EAE-4A0D-8EC1-89D9053C8FCB}">
-  <dimension ref="B3:L8"/>
+  <dimension ref="B3:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +581,7 @@
       <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -631,6 +643,55 @@
       </c>
       <c r="G8" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>